<commit_message>
Histograms for Org 2
</commit_message>
<xml_diff>
--- a/descriptive.xlsx
+++ b/descriptive.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,67 +436,97 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>OBSV_PreC_Location_G_other</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>OBSV_same_space_count_D_10p</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>OBSV_PreC_meetingsize0ffice_D_10plus</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>OBSV_Now_Interact_Work_within_org</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>OBSV_PreC_interative_B_remote</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Collaborative Work Enivornmental Preferences</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">Current Focused Work </t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Focused Work Environmental Preferences</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Office Satisfaction</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Pre Covid In Person Collab Work (1-3 people)</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Pre Covid In Person Collab Work (4-10+ people)</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Pre-Covid Hybrid Meetings</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Pre-Covid In Person Meetings</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Pre-Covid Remote Meetings</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Recommendations Questions</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Work Location Deciding Factors</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Work Satisf Features</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Future Workplace Features Preference</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Environment Productivity Impact</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Workplace Tech Features Importance</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Workplace Preference</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Office Workspace Preference</t>
         </is>
       </c>
     </row>
@@ -516,7 +546,7 @@
         <v>713</v>
       </c>
       <c r="E2" t="n">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="F2" t="n">
         <v>713</v>
@@ -543,6 +573,24 @@
         <v>713</v>
       </c>
       <c r="N2" t="n">
+        <v>713</v>
+      </c>
+      <c r="O2" t="n">
+        <v>713</v>
+      </c>
+      <c r="P2" t="n">
+        <v>713</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>713</v>
+      </c>
+      <c r="R2" t="n">
+        <v>713</v>
+      </c>
+      <c r="S2" t="n">
+        <v>713</v>
+      </c>
+      <c r="T2" t="n">
         <v>713</v>
       </c>
     </row>
@@ -553,43 +601,61 @@
         </is>
       </c>
       <c r="B3" t="n">
+        <v>0.6719200561009818</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.7095826426962472</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.2044419955920657</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.1501680322373501</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.8729593267882189</v>
+      </c>
+      <c r="G3" t="n">
         <v>5.349021875292828</v>
       </c>
-      <c r="C3" t="n">
-        <v>0.6781671348314607</v>
-      </c>
-      <c r="D3" t="n">
+      <c r="H3" t="n">
+        <v>0.8504638108155419</v>
+      </c>
+      <c r="I3" t="n">
         <v>4.084950709134868</v>
       </c>
-      <c r="E3" t="n">
+      <c r="J3" t="n">
         <v>4.122002820874472</v>
       </c>
-      <c r="F3" t="n">
-        <v>0.328132087159746</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.3579323308270677</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.3818215789473685</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.5043938811188812</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.2276396475770925</v>
-      </c>
       <c r="K3" t="n">
+        <v>0.2995980052993433</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.3589675994399235</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.358924131181476</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.4719637261585272</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.2856462039980057</v>
+      </c>
+      <c r="P3" t="n">
         <v>2.202516432955356</v>
       </c>
-      <c r="L3" t="n">
+      <c r="Q3" t="n">
         <v>2.471004243281471</v>
       </c>
-      <c r="M3" t="n">
+      <c r="R3" t="n">
         <v>4.334273624823695</v>
       </c>
-      <c r="N3" t="n">
+      <c r="S3" t="n">
         <v>0.3784001611928269</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0.1876065794848072</v>
       </c>
     </row>
     <row r="4">
@@ -599,43 +665,61 @@
         </is>
       </c>
       <c r="B4" t="n">
+        <v>0.4689307590702963</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.4251315873051083</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.374351734506099</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.2503496512593084</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.2831996551757824</v>
+      </c>
+      <c r="G4" t="n">
         <v>1.50337978108837</v>
       </c>
-      <c r="C4" t="n">
-        <v>0.2223859798463929</v>
-      </c>
-      <c r="D4" t="n">
+      <c r="H4" t="n">
+        <v>0.2500109680649201</v>
+      </c>
+      <c r="I4" t="n">
         <v>1.498473441905509</v>
       </c>
-      <c r="E4" t="n">
+      <c r="J4" t="n">
         <v>0.8013303159577678</v>
       </c>
-      <c r="F4" t="n">
-        <v>0.1292212116744064</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.2349537534099986</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.2539273389406653</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.2747413128248647</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.2039245812558415</v>
-      </c>
       <c r="K4" t="n">
+        <v>0.1428528832329196</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.2793626181254321</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.2707302378835066</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.2974585252053411</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.3646232645609411</v>
+      </c>
+      <c r="P4" t="n">
         <v>0.2965698816144888</v>
       </c>
-      <c r="L4" t="n">
+      <c r="Q4" t="n">
         <v>1.166024454252978</v>
       </c>
-      <c r="M4" t="n">
+      <c r="R4" t="n">
         <v>0.7669225226722741</v>
       </c>
-      <c r="N4" t="n">
+      <c r="S4" t="n">
         <v>0.247293969853232</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.05312349050094685</v>
       </c>
     </row>
     <row r="5">
@@ -645,16 +729,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>-2.220446049250313e-16</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>-2.220446049250313e-16</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -669,19 +753,37 @@
         <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
         <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5" t="n">
         <v>0</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" t="n">
+        <v>1</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.1666666666666666</v>
       </c>
     </row>
     <row r="6">
@@ -691,43 +793,61 @@
         </is>
       </c>
       <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
         <v>4.482344266190199</v>
       </c>
-      <c r="C6" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D6" t="n">
+      <c r="H6" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="I6" t="n">
         <v>3.142857142857143</v>
       </c>
-      <c r="E6" t="n">
+      <c r="J6" t="n">
         <v>4</v>
       </c>
-      <c r="F6" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="G6" t="n">
+      <c r="K6" t="n">
+        <v>0.2222222222222222</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.1176470588235294</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="N6" t="n">
         <v>0.2</v>
       </c>
-      <c r="H6" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="K6" t="n">
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" t="n">
         <v>1.939956595129009</v>
       </c>
-      <c r="L6" t="n">
+      <c r="Q6" t="n">
         <v>1.666666666666667</v>
       </c>
-      <c r="M6" t="n">
+      <c r="R6" t="n">
         <v>4</v>
       </c>
-      <c r="N6" t="n">
+      <c r="S6" t="n">
         <v>0.1428571428571428</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -737,43 +857,61 @@
         </is>
       </c>
       <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" t="n">
         <v>5.428571428571429</v>
       </c>
-      <c r="C7" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="D7" t="n">
+      <c r="H7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" t="n">
         <v>4.084950709134867</v>
       </c>
-      <c r="E7" t="n">
+      <c r="J7" t="n">
         <v>4</v>
       </c>
-      <c r="F7" t="n">
-        <v>0.328132087159746</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.3579323308270677</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.3818215789473685</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.5043938811188812</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.2276396475770925</v>
-      </c>
       <c r="K7" t="n">
+        <v>0.2995980052993432</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.3589675994399235</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.4719637261585272</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="P7" t="n">
         <v>2.164324610752314</v>
       </c>
-      <c r="L7" t="n">
+      <c r="Q7" t="n">
         <v>2.5</v>
       </c>
-      <c r="M7" t="n">
+      <c r="R7" t="n">
         <v>4.5</v>
       </c>
-      <c r="N7" t="n">
+      <c r="S7" t="n">
         <v>0.2857142857142857</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="8">
@@ -783,43 +921,61 @@
         </is>
       </c>
       <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" t="n">
         <v>6.285714285714286</v>
       </c>
-      <c r="C8" t="n">
-        <v>0.875</v>
-      </c>
-      <c r="D8" t="n">
+      <c r="H8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" t="n">
         <v>5</v>
       </c>
-      <c r="E8" t="n">
+      <c r="J8" t="n">
         <v>5</v>
       </c>
-      <c r="F8" t="n">
+      <c r="K8" t="n">
         <v>0.4</v>
       </c>
-      <c r="G8" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="H8" t="n">
+      <c r="L8" t="n">
         <v>0.5</v>
       </c>
-      <c r="I8" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.2276396475770925</v>
-      </c>
-      <c r="K8" t="n">
+      <c r="M8" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.7000000000000001</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="P8" t="n">
         <v>2.384615384615385</v>
       </c>
-      <c r="L8" t="n">
+      <c r="Q8" t="n">
         <v>3.333333333333333</v>
       </c>
-      <c r="M8" t="n">
+      <c r="R8" t="n">
         <v>5</v>
       </c>
-      <c r="N8" t="n">
+      <c r="S8" t="n">
         <v>0.5714285714285714</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="9">
@@ -829,43 +985,61 @@
         </is>
       </c>
       <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" t="n">
         <v>10</v>
       </c>
-      <c r="C9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" t="n">
+      <c r="H9" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" t="n">
         <v>10</v>
       </c>
-      <c r="E9" t="n">
+      <c r="J9" t="n">
         <v>5</v>
       </c>
-      <c r="F9" t="n">
-        <v>0.6714932562620424</v>
-      </c>
-      <c r="G9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I9" t="n">
-        <v>1</v>
-      </c>
-      <c r="J9" t="n">
-        <v>1</v>
-      </c>
       <c r="K9" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L9" t="n">
+        <v>1</v>
+      </c>
+      <c r="M9" t="n">
+        <v>1</v>
+      </c>
+      <c r="N9" t="n">
+        <v>1</v>
+      </c>
+      <c r="O9" t="n">
+        <v>1</v>
+      </c>
+      <c r="P9" t="n">
         <v>2.846153846153846</v>
       </c>
-      <c r="L9" t="n">
+      <c r="Q9" t="n">
         <v>5</v>
       </c>
-      <c r="M9" t="n">
+      <c r="R9" t="n">
         <v>5</v>
       </c>
-      <c r="N9" t="n">
-        <v>1</v>
+      <c r="S9" t="n">
+        <v>1</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0.3221891441597311</v>
       </c>
     </row>
   </sheetData>

</xml_diff>